<commit_message>
added tests for examples
</commit_message>
<xml_diff>
--- a/tbx/examples/data/data_provider_example.xlsx
+++ b/tbx/examples/data/data_provider_example.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mathworks-my.sharepoint.com/personal/ebenetce_mathworks_com/Documents/AEProjects/Climate/Public_SBTi/SBTi_MATLAB/examples/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\src\SBTi\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_44AC2284A3464F94CA1DDCAA48595A32695C8879" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{954B081A-A21D-482E-8650-17018DEDFD6C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -586,8 +585,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,64 +662,54 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q51" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:Q51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q51" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:Q51"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="company_name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="company_id"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="isic"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="country"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="region"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="industry_level_1"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="industry_level_2"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="industry_level_3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="industry_level_4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="sector"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ghg_s1s2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ghg_s3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="company_revenue"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="company_market_cap"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="company_enterprise_value"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="company_total_assets" dataDxfId="0">
+    <tableColumn id="1" name="company_name"/>
+    <tableColumn id="2" name="company_id"/>
+    <tableColumn id="3" name="isic"/>
+    <tableColumn id="4" name="country"/>
+    <tableColumn id="20" name="region"/>
+    <tableColumn id="5" name="industry_level_1"/>
+    <tableColumn id="22" name="industry_level_2"/>
+    <tableColumn id="21" name="industry_level_3"/>
+    <tableColumn id="7" name="industry_level_4"/>
+    <tableColumn id="6" name="sector"/>
+    <tableColumn id="18" name="ghg_s1s2"/>
+    <tableColumn id="8" name="ghg_s3"/>
+    <tableColumn id="9" name="company_revenue"/>
+    <tableColumn id="10" name="company_market_cap"/>
+    <tableColumn id="11" name="company_enterprise_value"/>
+    <tableColumn id="12" name="company_total_assets" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[company_market_cap]]*Q2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="company_cash_equivalents"/>
+    <tableColumn id="13" name="company_cash_equivalents"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:P120" totalsRowShown="0">
-  <autoFilter ref="A1:P120" xr:uid="{00000000-0009-0000-0100-000002000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="CA0000000019"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table4" displayName="Table4" ref="A1:P120" totalsRowShown="0">
+  <autoFilter ref="A1:P120"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="company_name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="company_id"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="target_type"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="intensity_metric"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="scope"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="coverage_s1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="coverage_s2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="coverage_s3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="reduction_ambition"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="base_year"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="end_year"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="start_year"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="base_year_ghg_s1"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="base_year_ghg_s2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="base_year_ghg_s3"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="achieved_reduction"/>
+    <tableColumn id="1" name="company_name"/>
+    <tableColumn id="2" name="company_id"/>
+    <tableColumn id="3" name="target_type"/>
+    <tableColumn id="10" name="intensity_metric"/>
+    <tableColumn id="4" name="scope"/>
+    <tableColumn id="12" name="coverage_s1"/>
+    <tableColumn id="11" name="coverage_s2"/>
+    <tableColumn id="5" name="coverage_s3"/>
+    <tableColumn id="6" name="reduction_ambition"/>
+    <tableColumn id="7" name="base_year"/>
+    <tableColumn id="8" name="end_year"/>
+    <tableColumn id="9" name="start_year"/>
+    <tableColumn id="13" name="base_year_ghg_s1"/>
+    <tableColumn id="14" name="base_year_ghg_s2"/>
+    <tableColumn id="15" name="base_year_ghg_s3"/>
+    <tableColumn id="16" name="achieved_reduction"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -988,14 +977,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1008,7 +997,7 @@
     <col min="17" max="17" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1050,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -1099,7 +1088,7 @@
         <v>4528467714.7267609</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -1137,7 +1126,7 @@
         <v>69006940.998092517</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -1175,7 +1164,7 @@
         <v>1163119848.4230556</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>170</v>
       </c>
@@ -1213,7 +1202,7 @@
         <v>117630751.45422383</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>171</v>
       </c>
@@ -1251,7 +1240,7 @@
         <v>28933197273.168182</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -1289,7 +1278,7 @@
         <v>51876930016.314178</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>173</v>
       </c>
@@ -1327,7 +1316,7 @@
         <v>2214490.9702577037</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -1365,7 +1354,7 @@
         <v>203940251.11854151</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>175</v>
       </c>
@@ -1403,7 +1392,7 @@
         <v>42950453116.50563</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>176</v>
       </c>
@@ -1441,7 +1430,7 @@
         <v>5520000408.4878492</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>177</v>
       </c>
@@ -1479,7 +1468,7 @@
         <v>505519258.45795137</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>178</v>
       </c>
@@ -1517,7 +1506,7 @@
         <v>462245314.11453331</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>179</v>
       </c>
@@ -1555,7 +1544,7 @@
         <v>1853875026.0311818</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -1593,7 +1582,7 @@
         <v>3272481697.8285317</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -1631,7 +1620,7 @@
         <v>518880676.89759755</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>182</v>
       </c>
@@ -1669,7 +1658,7 @@
         <v>990719858.47337103</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>184</v>
       </c>
@@ -1707,7 +1696,7 @@
         <v>470283632.88013947</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1745,7 +1734,7 @@
         <v>963039844.50366735</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1783,7 +1772,7 @@
         <v>23467516.32994597</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1821,7 +1810,7 @@
         <v>457926390.7271148</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1859,7 +1848,7 @@
         <v>469617764.24836379</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1897,7 +1886,7 @@
         <v>209706066.63280141</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1935,7 +1924,7 @@
         <v>80140338.552216381</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1973,7 +1962,7 @@
         <v>1863069356.1369269</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2011,7 +2000,7 @@
         <v>802015633.4125073</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2049,7 +2038,7 @@
         <v>1090445581.1975896</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -2087,7 +2076,7 @@
         <v>408632883.32140654</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2125,7 +2114,7 @@
         <v>223357269.54921383</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -2163,7 +2152,7 @@
         <v>1279584288.1275206</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -2201,7 +2190,7 @@
         <v>259739897.26190066</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -2239,7 +2228,7 @@
         <v>2957267010.5849843</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -2277,7 +2266,7 @@
         <v>3249873922.9934068</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2315,7 +2304,7 @@
         <v>1054147392.1400725</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2353,7 +2342,7 @@
         <v>16164035.009301951</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -2391,7 +2380,7 @@
         <v>76375335.415532187</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -2429,7 +2418,7 @@
         <v>403556882.32980388</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -2467,7 +2456,7 @@
         <v>359922992.06079412</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -2505,7 +2494,7 @@
         <v>188775849.06628573</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -2543,7 +2532,7 @@
         <v>3126017043.1166129</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -2581,7 +2570,7 @@
         <v>25963862784.153816</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -2619,7 +2608,7 @@
         <v>216444951.50947747</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -2657,7 +2646,7 @@
         <v>463981837.16979945</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -2695,7 +2684,7 @@
         <v>630827983.47226107</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -2733,7 +2722,7 @@
         <v>1089931685.5934117</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -2771,7 +2760,7 @@
         <v>1580248549.8247914</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>108</v>
       </c>
@@ -2809,7 +2798,7 @@
         <v>360167278.93933254</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>112</v>
       </c>
@@ -2847,7 +2836,7 @@
         <v>23659060554.326973</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>115</v>
       </c>
@@ -2885,7 +2874,7 @@
         <v>94976895574.746582</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>118</v>
       </c>
@@ -2923,7 +2912,7 @@
         <v>408452279.29417968</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>183</v>
       </c>
@@ -2971,14 +2960,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -2992,7 +2979,7 @@
     <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3042,7 +3029,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -3083,7 +3070,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -3128,7 +3115,7 @@
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" hidden="1">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -3169,7 +3156,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>170</v>
       </c>
@@ -3216,7 +3203,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>171</v>
       </c>
@@ -3263,7 +3250,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -3307,7 +3294,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:17" hidden="1">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>173</v>
       </c>
@@ -3345,7 +3332,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -3389,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>175</v>
       </c>
@@ -3433,7 +3420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>176</v>
       </c>
@@ -3477,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>177</v>
       </c>
@@ -3518,7 +3505,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>178</v>
       </c>
@@ -3559,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>179</v>
       </c>
@@ -3600,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -3641,7 +3628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -3682,7 +3669,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:16" hidden="1">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>182</v>
       </c>
@@ -3723,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" hidden="1">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>184</v>
       </c>
@@ -3761,7 +3748,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="19" spans="1:16" hidden="1">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -3799,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" hidden="1">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -3837,7 +3824,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" hidden="1">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3875,7 +3862,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:16" hidden="1">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -3913,7 +3900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" hidden="1">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -3951,7 +3938,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:16" hidden="1">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -3992,7 +3979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -4033,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" hidden="1">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -4074,7 +4061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" hidden="1">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -4118,7 +4105,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:16" hidden="1">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -4153,7 +4140,7 @@
         <v>0.49600000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:16" hidden="1">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -4194,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" hidden="1">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -4235,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" hidden="1">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -4276,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -4317,7 +4304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -4355,7 +4342,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -4396,7 +4383,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -4431,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -4472,7 +4459,7 @@
         <v>6.1699999999999998E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" hidden="1">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -4513,7 +4500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" hidden="1">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -4554,7 +4541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" hidden="1">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -4592,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" hidden="1">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -4630,7 +4617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" hidden="1">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -4674,7 +4661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" hidden="1">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -4718,7 +4705,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="43" spans="1:16" hidden="1">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -4759,7 +4746,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="44" spans="1:16" hidden="1">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>121</v>
       </c>
@@ -4800,7 +4787,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="45" spans="1:16" hidden="1">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>168</v>
       </c>
@@ -4841,7 +4828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" hidden="1">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>169</v>
       </c>
@@ -4885,7 +4872,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="47" spans="1:16" hidden="1">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -4929,7 +4916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>171</v>
       </c>
@@ -4970,7 +4957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" hidden="1">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>172</v>
       </c>
@@ -5014,7 +5001,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>173</v>
       </c>
@@ -5061,7 +5048,7 @@
         <v>0.35799999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>174</v>
       </c>
@@ -5102,7 +5089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16" hidden="1">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>175</v>
       </c>
@@ -5143,7 +5130,7 @@
         <v>0.32600000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>176</v>
       </c>
@@ -5187,7 +5174,7 @@
         <v>5.4000000000000006E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:16" hidden="1">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>177</v>
       </c>
@@ -5228,7 +5215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" hidden="1">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>178</v>
       </c>
@@ -5269,7 +5256,7 @@
         <v>0.30809999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:16" hidden="1">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>179</v>
       </c>
@@ -5310,7 +5297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" hidden="1">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>180</v>
       </c>
@@ -5351,7 +5338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" hidden="1">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>181</v>
       </c>
@@ -5392,7 +5379,7 @@
         <v>0.41000000000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:16" hidden="1">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>182</v>
       </c>
@@ -5436,7 +5423,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="60" spans="1:16" hidden="1">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>184</v>
       </c>
@@ -5480,7 +5467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" hidden="1">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>81</v>
       </c>
@@ -5524,7 +5511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>83</v>
       </c>
@@ -5565,7 +5552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" hidden="1">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -5606,7 +5593,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="64" spans="1:16" hidden="1">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -5647,7 +5634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:16" hidden="1">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>90</v>
       </c>
@@ -5691,7 +5678,7 @@
         <v>0.47789999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:16" hidden="1">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -5735,7 +5722,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>83</v>
       </c>
@@ -5776,7 +5763,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="68" spans="1:16" hidden="1">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -5820,7 +5807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:16" hidden="1">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -5858,7 +5845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" hidden="1">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>90</v>
       </c>
@@ -5899,7 +5886,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:16" hidden="1">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -5943,7 +5930,7 @@
         <v>6.4100000000000004E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -5984,7 +5971,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:16" hidden="1">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -6025,7 +6012,7 @@
         <v>0.11220000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:16" hidden="1">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -6069,7 +6056,7 @@
         <v>0.22870000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:16" hidden="1">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -6110,7 +6097,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:16" hidden="1">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>40</v>
       </c>
@@ -6154,7 +6141,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:16" hidden="1">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>43</v>
       </c>
@@ -6198,7 +6185,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="78" spans="1:16" hidden="1">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>53</v>
       </c>
@@ -6242,7 +6229,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="79" spans="1:16" hidden="1">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>121</v>
       </c>
@@ -6280,7 +6267,7 @@
         <v>0.84400000000000008</v>
       </c>
     </row>
-    <row r="80" spans="1:16" hidden="1">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>168</v>
       </c>
@@ -6327,7 +6314,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:16" hidden="1">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -6371,7 +6358,7 @@
         <v>0.55670000000000008</v>
       </c>
     </row>
-    <row r="82" spans="1:16" hidden="1">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>170</v>
       </c>
@@ -6412,7 +6399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" hidden="1">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>171</v>
       </c>
@@ -6453,7 +6440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" hidden="1">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>172</v>
       </c>
@@ -6494,7 +6481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16" hidden="1">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>173</v>
       </c>
@@ -6535,7 +6522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" hidden="1">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>174</v>
       </c>
@@ -6573,7 +6560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:16" hidden="1">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>175</v>
       </c>
@@ -6617,7 +6604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:16" hidden="1">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>176</v>
       </c>
@@ -6655,7 +6642,7 @@
         <v>0.36700000000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:16" hidden="1">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>178</v>
       </c>
@@ -6696,7 +6683,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="90" spans="1:16" hidden="1">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>180</v>
       </c>
@@ -6734,7 +6721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" hidden="1">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -6772,7 +6759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" hidden="1">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>181</v>
       </c>
@@ -6810,7 +6797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:16" hidden="1">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>181</v>
       </c>
@@ -6848,7 +6835,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="94" spans="1:16" hidden="1">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>184</v>
       </c>
@@ -6889,7 +6876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:16" hidden="1">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>121</v>
       </c>
@@ -6930,7 +6917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" hidden="1">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>168</v>
       </c>
@@ -6974,7 +6961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" hidden="1">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>169</v>
       </c>
@@ -7018,7 +7005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:16" hidden="1">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>170</v>
       </c>
@@ -7056,7 +7043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" hidden="1">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>170</v>
       </c>
@@ -7094,7 +7081,7 @@
         <v>0.82000000000000006</v>
       </c>
     </row>
-    <row r="100" spans="1:16" hidden="1">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>172</v>
       </c>
@@ -7138,7 +7125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" hidden="1">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>173</v>
       </c>
@@ -7176,7 +7163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16" hidden="1">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>174</v>
       </c>
@@ -7217,7 +7204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:16" hidden="1">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>175</v>
       </c>
@@ -7261,7 +7248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" hidden="1">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>176</v>
       </c>
@@ -7305,7 +7292,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:16" hidden="1">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>177</v>
       </c>
@@ -7346,7 +7333,7 @@
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="106" spans="1:16" hidden="1">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>178</v>
       </c>
@@ -7390,7 +7377,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="107" spans="1:16" hidden="1">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>179</v>
       </c>
@@ -7431,7 +7418,7 @@
         <v>0.69000000000000006</v>
       </c>
     </row>
-    <row r="108" spans="1:16" hidden="1">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>180</v>
       </c>
@@ -7472,7 +7459,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="109" spans="1:16" hidden="1">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>181</v>
       </c>
@@ -7516,7 +7503,7 @@
         <v>0.57020000000000004</v>
       </c>
     </row>
-    <row r="110" spans="1:16" hidden="1">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>182</v>
       </c>
@@ -7557,7 +7544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" hidden="1">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>184</v>
       </c>
@@ -7598,7 +7585,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>83</v>
       </c>
@@ -7639,7 +7626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" hidden="1">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>85</v>
       </c>
@@ -7680,7 +7667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" hidden="1">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>88</v>
       </c>
@@ -7721,7 +7708,7 @@
         <v>1.52E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:16" hidden="1">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>90</v>
       </c>
@@ -7762,7 +7749,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:16" hidden="1">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>81</v>
       </c>
@@ -7803,7 +7790,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>83</v>
       </c>
@@ -7847,7 +7834,7 @@
         <v>0.154</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>83</v>
       </c>
@@ -7891,7 +7878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>83</v>
       </c>
@@ -7932,7 +7919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>83</v>
       </c>

</xml_diff>